<commit_message>
bug fixes and lols
</commit_message>
<xml_diff>
--- a/conversations.xlsx
+++ b/conversations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brettpietruszka/Documents/gt/ConversationScript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570106FA-6BBE-A64A-9333-D1D97A010AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BB5A1F-3DB6-B644-9FFC-F2F4E4603FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -239,7 +239,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -259,6 +259,12 @@
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -383,10 +389,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -420,8 +427,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -637,14 +646,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W973"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="4.85546875" customWidth="1"/>
@@ -728,7 +737,7 @@
       <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="33"/>
       <c r="C2" s="11" t="s">
         <v>15</v>
       </c>
@@ -764,7 +773,7 @@
       <c r="O2" s="10"/>
       <c r="P2" s="16">
         <f t="shared" ref="P2:P53" ca="1" si="0">RANDBETWEEN(DATE($Q$1,$R$1,$S$1),DATE($Q$1,$T$1,$U$1))</f>
-        <v>44571</v>
+        <v>44576</v>
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="10"/>
@@ -773,7 +782,7 @@
       <c r="U2" s="10"/>
       <c r="V2" s="10">
         <f t="shared" ref="V2:V53" ca="1" si="1">INDEX(N:N, RANDBETWEEN(0,2), 0)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W2" s="10"/>
     </row>
@@ -817,7 +826,7 @@
       <c r="O3" s="10"/>
       <c r="P3" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44574</v>
+        <v>44570</v>
       </c>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
@@ -826,7 +835,7 @@
       <c r="U3" s="10"/>
       <c r="V3" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W3" s="10"/>
     </row>
@@ -869,7 +878,7 @@
       <c r="O4" s="10"/>
       <c r="P4" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44578</v>
+        <v>44576</v>
       </c>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
@@ -878,7 +887,7 @@
       <c r="U4" s="10"/>
       <c r="V4" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W4" s="10"/>
     </row>
@@ -919,7 +928,7 @@
       <c r="O5" s="10"/>
       <c r="P5" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44575</v>
+        <v>44571</v>
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
@@ -969,7 +978,7 @@
       <c r="O6" s="10"/>
       <c r="P6" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44572</v>
       </c>
       <c r="Q6" s="10"/>
       <c r="R6" s="10"/>
@@ -978,7 +987,7 @@
       <c r="U6" s="10"/>
       <c r="V6" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W6" s="10"/>
     </row>
@@ -1019,7 +1028,7 @@
       <c r="O7" s="10"/>
       <c r="P7" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44569</v>
+        <v>44580</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
@@ -1069,7 +1078,7 @@
       <c r="O8" s="10"/>
       <c r="P8" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44582</v>
+        <v>44572</v>
       </c>
       <c r="Q8" s="10"/>
       <c r="R8" s="10"/>
@@ -1078,7 +1087,7 @@
       <c r="U8" s="10"/>
       <c r="V8" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W8" s="10"/>
     </row>
@@ -1119,7 +1128,7 @@
       <c r="O9" s="10"/>
       <c r="P9" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44570</v>
+        <v>44572</v>
       </c>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
@@ -1128,7 +1137,7 @@
       <c r="U9" s="10"/>
       <c r="V9" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W9" s="10"/>
     </row>
@@ -1167,7 +1176,7 @@
       <c r="O10" s="10"/>
       <c r="P10" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44569</v>
+        <v>44574</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -1176,7 +1185,7 @@
       <c r="U10" s="10"/>
       <c r="V10" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="10"/>
     </row>
@@ -1215,7 +1224,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44582</v>
       </c>
       <c r="Q11" s="10"/>
       <c r="R11" s="10"/>
@@ -1224,7 +1233,7 @@
       <c r="U11" s="10"/>
       <c r="V11" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W11" s="10"/>
     </row>
@@ -1267,7 +1276,7 @@
       <c r="O12" s="10"/>
       <c r="P12" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44579</v>
+        <v>44582</v>
       </c>
       <c r="Q12" s="10"/>
       <c r="R12" s="10"/>
@@ -1276,7 +1285,7 @@
       <c r="U12" s="10"/>
       <c r="V12" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W12" s="10"/>
     </row>
@@ -1317,7 +1326,7 @@
       <c r="O13" s="10"/>
       <c r="P13" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44576</v>
+        <v>44584</v>
       </c>
       <c r="Q13" s="10"/>
       <c r="R13" s="10"/>
@@ -1367,7 +1376,7 @@
       <c r="O14" s="10"/>
       <c r="P14" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44571</v>
+        <v>44572</v>
       </c>
       <c r="Q14" s="10"/>
       <c r="R14" s="10"/>
@@ -1376,7 +1385,7 @@
       <c r="U14" s="10"/>
       <c r="V14" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W14" s="10"/>
     </row>
@@ -1417,7 +1426,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44582</v>
+        <v>44570</v>
       </c>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -1467,7 +1476,7 @@
       <c r="O16" s="10"/>
       <c r="P16" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44576</v>
+        <v>44571</v>
       </c>
       <c r="Q16" s="10"/>
       <c r="R16" s="10"/>
@@ -1476,7 +1485,7 @@
       <c r="U16" s="10"/>
       <c r="V16" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="10"/>
     </row>
@@ -1519,7 +1528,7 @@
       <c r="O17" s="10"/>
       <c r="P17" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44584</v>
       </c>
       <c r="Q17" s="10"/>
       <c r="R17" s="10"/>
@@ -1528,7 +1537,7 @@
       <c r="U17" s="10"/>
       <c r="V17" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="10"/>
     </row>
@@ -1569,7 +1578,7 @@
       <c r="O18" s="10"/>
       <c r="P18" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44581</v>
+        <v>44585</v>
       </c>
       <c r="Q18" s="10"/>
       <c r="R18" s="10"/>
@@ -1619,7 +1628,7 @@
       <c r="O19" s="10"/>
       <c r="P19" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44583</v>
+        <v>44580</v>
       </c>
       <c r="Q19" s="10"/>
       <c r="R19" s="10"/>
@@ -1628,7 +1637,7 @@
       <c r="U19" s="10"/>
       <c r="V19" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W19" s="10"/>
     </row>
@@ -1667,7 +1676,7 @@
       <c r="O20" s="10"/>
       <c r="P20" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44579</v>
       </c>
       <c r="Q20" s="10"/>
       <c r="R20" s="10"/>
@@ -1676,7 +1685,7 @@
       <c r="U20" s="10"/>
       <c r="V20" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W20" s="10"/>
     </row>
@@ -1717,7 +1726,7 @@
       <c r="O21" s="10"/>
       <c r="P21" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44576</v>
+        <v>44569</v>
       </c>
       <c r="Q21" s="10"/>
       <c r="R21" s="10"/>
@@ -1767,7 +1776,7 @@
       <c r="O22" s="10"/>
       <c r="P22" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44577</v>
+        <v>44585</v>
       </c>
       <c r="Q22" s="10"/>
       <c r="R22" s="10"/>
@@ -1776,7 +1785,7 @@
       <c r="U22" s="10"/>
       <c r="V22" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W22" s="10"/>
     </row>
@@ -1817,7 +1826,7 @@
       <c r="O23" s="10"/>
       <c r="P23" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44570</v>
+        <v>44584</v>
       </c>
       <c r="Q23" s="10"/>
       <c r="R23" s="10"/>
@@ -1826,7 +1835,7 @@
       <c r="U23" s="10"/>
       <c r="V23" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W23" s="10"/>
     </row>
@@ -1917,7 +1926,7 @@
       <c r="O25" s="10"/>
       <c r="P25" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44575</v>
+        <v>44585</v>
       </c>
       <c r="Q25" s="10"/>
       <c r="R25" s="10"/>
@@ -1926,7 +1935,7 @@
       <c r="U25" s="10"/>
       <c r="V25" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W25" s="10"/>
     </row>
@@ -1967,7 +1976,7 @@
       <c r="O26" s="10"/>
       <c r="P26" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44582</v>
+        <v>44576</v>
       </c>
       <c r="Q26" s="10"/>
       <c r="R26" s="10"/>
@@ -1976,7 +1985,7 @@
       <c r="U26" s="10"/>
       <c r="V26" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W26" s="10"/>
     </row>
@@ -2017,7 +2026,7 @@
       <c r="O27" s="10"/>
       <c r="P27" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44579</v>
+        <v>44583</v>
       </c>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -2026,7 +2035,7 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W27" s="10"/>
     </row>
@@ -2067,7 +2076,7 @@
       <c r="O28" s="10"/>
       <c r="P28" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44575</v>
       </c>
       <c r="Q28" s="10"/>
       <c r="R28" s="10"/>
@@ -2076,7 +2085,7 @@
       <c r="U28" s="10"/>
       <c r="V28" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W28" s="10"/>
     </row>
@@ -2115,7 +2124,7 @@
       <c r="O29" s="10"/>
       <c r="P29" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44569</v>
+        <v>44577</v>
       </c>
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
@@ -2124,7 +2133,7 @@
       <c r="U29" s="10"/>
       <c r="V29" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W29" s="10"/>
     </row>
@@ -2163,7 +2172,7 @@
       <c r="O30" s="10"/>
       <c r="P30" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44584</v>
+        <v>44579</v>
       </c>
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
@@ -2172,7 +2181,7 @@
       <c r="U30" s="10"/>
       <c r="V30" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W30" s="10"/>
     </row>
@@ -2210,7 +2219,7 @@
       <c r="O31" s="10"/>
       <c r="P31" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44570</v>
+        <v>44580</v>
       </c>
       <c r="Q31" s="10"/>
       <c r="R31" s="10"/>
@@ -2219,7 +2228,7 @@
       <c r="U31" s="10"/>
       <c r="V31" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W31" s="10"/>
     </row>
@@ -2257,7 +2266,7 @@
       <c r="O32" s="10"/>
       <c r="P32" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44583</v>
+        <v>44579</v>
       </c>
       <c r="Q32" s="10"/>
       <c r="R32" s="10"/>
@@ -2266,7 +2275,7 @@
       <c r="U32" s="10"/>
       <c r="V32" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W32" s="10"/>
     </row>
@@ -2304,7 +2313,7 @@
       <c r="O33" s="10"/>
       <c r="P33" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44583</v>
+        <v>44571</v>
       </c>
       <c r="Q33" s="10"/>
       <c r="R33" s="10"/>
@@ -2313,7 +2322,7 @@
       <c r="U33" s="10"/>
       <c r="V33" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33" s="10"/>
     </row>
@@ -2352,7 +2361,7 @@
       <c r="O34" s="10"/>
       <c r="P34" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44580</v>
+        <v>44572</v>
       </c>
       <c r="Q34" s="10"/>
       <c r="R34" s="10"/>
@@ -2361,7 +2370,7 @@
       <c r="U34" s="10"/>
       <c r="V34" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W34" s="10"/>
     </row>
@@ -2400,7 +2409,7 @@
       <c r="O35" s="10"/>
       <c r="P35" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="Q35" s="10"/>
       <c r="R35" s="10"/>
@@ -2450,7 +2459,7 @@
       <c r="O36" s="10"/>
       <c r="P36" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44581</v>
       </c>
       <c r="Q36" s="10"/>
       <c r="R36" s="10"/>
@@ -2507,7 +2516,7 @@
       <c r="U37" s="10"/>
       <c r="V37" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W37" s="10"/>
     </row>
@@ -2546,7 +2555,7 @@
       <c r="O38" s="10"/>
       <c r="P38" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44580</v>
+        <v>44569</v>
       </c>
       <c r="Q38" s="10"/>
       <c r="R38" s="10"/>
@@ -2596,7 +2605,7 @@
       <c r="O39" s="10"/>
       <c r="P39" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44573</v>
+        <v>44583</v>
       </c>
       <c r="Q39" s="10"/>
       <c r="R39" s="10"/>
@@ -2644,7 +2653,7 @@
       <c r="O40" s="10"/>
       <c r="P40" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44583</v>
+        <v>44574</v>
       </c>
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
@@ -2653,7 +2662,7 @@
       <c r="U40" s="10"/>
       <c r="V40" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W40" s="10"/>
     </row>
@@ -2692,7 +2701,7 @@
       <c r="O41" s="10"/>
       <c r="P41" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44580</v>
+        <v>44584</v>
       </c>
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
@@ -2701,7 +2710,7 @@
       <c r="U41" s="10"/>
       <c r="V41" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W41" s="10"/>
     </row>
@@ -2740,7 +2749,7 @@
       <c r="O42" s="10"/>
       <c r="P42" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44578</v>
+        <v>44569</v>
       </c>
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
@@ -2788,7 +2797,7 @@
       <c r="O43" s="10"/>
       <c r="P43" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44582</v>
       </c>
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
@@ -2838,7 +2847,7 @@
       <c r="O44" s="10"/>
       <c r="P44" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44577</v>
+        <v>44575</v>
       </c>
       <c r="Q44" s="10"/>
       <c r="R44" s="10"/>
@@ -2847,7 +2856,7 @@
       <c r="U44" s="10"/>
       <c r="V44" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W44" s="10"/>
     </row>
@@ -2886,7 +2895,7 @@
       <c r="O45" s="10"/>
       <c r="P45" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44581</v>
+        <v>44573</v>
       </c>
       <c r="Q45" s="10"/>
       <c r="R45" s="10"/>
@@ -2895,7 +2904,7 @@
       <c r="U45" s="10"/>
       <c r="V45" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W45" s="10"/>
     </row>
@@ -2934,7 +2943,7 @@
       <c r="O46" s="10"/>
       <c r="P46" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44569</v>
+        <v>44579</v>
       </c>
       <c r="Q46" s="10"/>
       <c r="R46" s="10"/>
@@ -2943,7 +2952,7 @@
       <c r="U46" s="10"/>
       <c r="V46" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W46" s="10"/>
     </row>
@@ -2982,7 +2991,7 @@
       <c r="O47" s="10"/>
       <c r="P47" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44576</v>
       </c>
       <c r="Q47" s="10"/>
       <c r="R47" s="10"/>
@@ -2991,7 +3000,7 @@
       <c r="U47" s="10"/>
       <c r="V47" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="10"/>
     </row>
@@ -3030,7 +3039,7 @@
       <c r="O48" s="10"/>
       <c r="P48" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44576</v>
+        <v>44583</v>
       </c>
       <c r="Q48" s="10"/>
       <c r="R48" s="10"/>
@@ -3039,7 +3048,7 @@
       <c r="U48" s="10"/>
       <c r="V48" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W48" s="10"/>
     </row>
@@ -3078,7 +3087,7 @@
       <c r="O49" s="10"/>
       <c r="P49" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44574</v>
+        <v>44579</v>
       </c>
       <c r="Q49" s="10"/>
       <c r="R49" s="10"/>
@@ -3087,7 +3096,7 @@
       <c r="U49" s="10"/>
       <c r="V49" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W49" s="10"/>
     </row>
@@ -3126,7 +3135,7 @@
       <c r="O50" s="10"/>
       <c r="P50" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44580</v>
+        <v>44582</v>
       </c>
       <c r="Q50" s="10"/>
       <c r="R50" s="10"/>
@@ -3135,7 +3144,7 @@
       <c r="U50" s="10"/>
       <c r="V50" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W50" s="10"/>
     </row>
@@ -3176,7 +3185,7 @@
       <c r="O51" s="10"/>
       <c r="P51" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44584</v>
+        <v>44579</v>
       </c>
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
@@ -3224,7 +3233,7 @@
       <c r="O52" s="10"/>
       <c r="P52" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44582</v>
+        <v>44579</v>
       </c>
       <c r="Q52" s="10"/>
       <c r="R52" s="10"/>
@@ -3272,7 +3281,7 @@
       <c r="O53" s="10"/>
       <c r="P53" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>44583</v>
+        <v>44572</v>
       </c>
       <c r="Q53" s="10"/>
       <c r="R53" s="10"/>

</xml_diff>